<commit_message>
Added configuration data into the code
</commit_message>
<xml_diff>
--- a/I710_networkConfig.xlsx
+++ b/I710_networkConfig.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Veh_Input" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="76">
   <si>
     <t>Input ID</t>
   </si>
@@ -105,9 +105,6 @@
     <t>14,15,16,17</t>
   </si>
   <si>
-    <t>18,19,20,21</t>
-  </si>
-  <si>
     <t>22,23,24,25</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>VSL (on ramp)</t>
+  </si>
+  <si>
+    <t>18,19,20,21,70</t>
   </si>
 </sst>
 </file>
@@ -339,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -350,7 +350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -359,20 +358,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -737,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,13 +979,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1065,7 @@
         <v>270</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,7 +1079,7 @@
         <v>282</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,638 +1117,638 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>11907.111000000001</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>84</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>11907.111000000001</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>4</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
         <v>1889.6559999999999</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>83</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1889.6559999999999</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>4</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1739.5119999999999</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>81</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>1739.5119999999999</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>1925.384</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>79</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1925.384</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>4</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="17">
         <v>2118.3719999999998</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>77</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>113.349</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>5</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="10">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="9">
         <v>76</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>2005.0229999999999</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>4</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="18">
         <v>5</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="18">
         <f>D8+D9</f>
         <v>2235.0100000000002</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>75</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>1905.79</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>4</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="10">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="9">
         <v>74</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>329.22</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>5</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="18">
         <v>6</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="18">
         <f>D10+D11</f>
         <v>2116.636</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>72</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>475.108</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>4</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="10">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="9">
         <v>70</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>1641.528</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>7</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <v>1991.1569999999999</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>69</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>1991.1569999999999</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>4</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="18">
         <v>8</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="18">
         <f>D13+D14</f>
         <v>2130.672</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>68</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>1952.8340000000001</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>4</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>52</v>
+      <c r="F13" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="10">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="9">
         <v>66</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>177.83799999999999</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <v>5</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>52</v>
+      <c r="F14" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>9</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>2921.1610000000001</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>65</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>2921.1610000000001</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>3</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="18">
         <v>10</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="18">
         <f>D16+D17+D18</f>
         <v>1611.075</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>63</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>180</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>4</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="10">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="9">
         <v>62</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>965.88499999999999</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>3</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="10">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="9">
         <v>60</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>465.19</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <v>4</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>11</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>1924.33</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>59</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>1924.33</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <v>3</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>12</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>2001.9970000000001</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>58</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>2001.9970000000001</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>3</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="18">
         <v>13</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="18">
         <f>D21+D22+D23</f>
         <v>1539.5240000000001</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>57</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>319.61200000000002</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>4</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="10">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="9">
         <v>55</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>736.15499999999997</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>3</v>
       </c>
-      <c r="F22" s="10"/>
+      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="10">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="9">
         <v>51</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>483.75700000000001</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="9">
         <v>4</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="A24" s="18">
         <v>14</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="18">
         <f>D24+D25+D26</f>
         <v>2131.9360000000001</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>50</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="9">
         <v>672.87900000000002</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>3</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="10">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="9">
         <v>19</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="9">
         <v>261.69299999999998</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>4</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="10">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="9">
         <v>18</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="9">
         <v>1197.364</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>3</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="17">
         <v>15</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="17">
         <v>1895.2080000000001</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>17</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="9">
         <v>1783.1010000000001</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <v>3</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="10">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="9">
         <v>339</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <v>112.107</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="9">
         <v>4</v>
       </c>
-      <c r="F28" s="10"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>16</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <v>1494.979</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <v>338</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="9">
         <v>1494.979</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>3</v>
       </c>
-      <c r="F29" s="10"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="17">
         <v>17</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="17">
         <v>2268.8890000000001</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>337</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <v>119.667</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="9">
         <v>4</v>
       </c>
-      <c r="F30" s="10"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="10">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="9">
         <v>310</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="9">
         <v>1299.337</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>3</v>
       </c>
-      <c r="F31" s="10"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="10">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="9">
         <v>311</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="9">
         <v>146.82400000000001</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>4</v>
       </c>
-      <c r="F32" s="10"/>
+      <c r="F32" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="10">
+      <c r="A33" s="17"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="9">
         <v>309</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="9">
         <v>228.541</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>3</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="10">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="9">
         <v>307</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <v>312.976</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="9">
         <v>4</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="10">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="9">
         <v>306</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <v>65.256</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="9">
         <v>3</v>
       </c>
-      <c r="F35" s="10"/>
+      <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="10">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="9">
         <v>304</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="9">
         <v>96.287999999999997</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="9">
         <v>5</v>
       </c>
-      <c r="F36" s="10"/>
+      <c r="F36" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -1751,20 +1757,20 @@
       <c r="A55" s="3"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -1804,497 +1810,607 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="9" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>0</v>
       </c>
       <c r="B2" s="15">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>83</v>
+      </c>
+      <c r="C3" s="11">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15">
+        <v>79</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15">
-        <v>2</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="E4" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="15">
+        <v>82</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>13</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="15">
+        <v>80</v>
+      </c>
+      <c r="C6" s="11">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11">
+        <v>77</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15">
+        <v>79</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15">
+        <v>76</v>
+      </c>
+      <c r="C8" s="11">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="15">
+        <v>78</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>18</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>5</v>
+      </c>
+      <c r="B10" s="15">
+        <v>72</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="15">
+        <v>73</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11">
+        <v>27</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>6</v>
+      </c>
+      <c r="B12" s="15">
+        <v>70</v>
+      </c>
+      <c r="C12" s="11">
+        <v>11</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15">
+        <v>71</v>
+      </c>
+      <c r="C13" s="11">
         <v>12</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D13" s="11">
+        <v>78</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>7</v>
+      </c>
+      <c r="B14" s="15">
+        <v>69</v>
+      </c>
+      <c r="C14" s="11">
+        <v>13</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15">
+        <v>65</v>
+      </c>
+      <c r="C15" s="11">
+        <v>14</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="15">
+        <v>67</v>
+      </c>
+      <c r="C16" s="11">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>9</v>
+      </c>
+      <c r="B17" s="15">
+        <v>65</v>
+      </c>
+      <c r="C17" s="11">
+        <v>16</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>10</v>
+      </c>
+      <c r="B18" s="15">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>2</v>
-      </c>
-      <c r="B4" s="15">
-        <v>3</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="C18" s="11">
+        <v>17</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="15">
+        <v>64</v>
+      </c>
+      <c r="C19" s="11">
+        <v>18</v>
+      </c>
+      <c r="D19" s="11">
+        <v>79</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="15">
         <v>61</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="15">
-        <v>4</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="C20" s="11">
+        <v>19</v>
+      </c>
+      <c r="D20" s="11">
+        <v>80</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>11</v>
+      </c>
+      <c r="B21" s="15">
+        <v>59</v>
+      </c>
+      <c r="C21" s="11">
+        <v>20</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>12</v>
+      </c>
+      <c r="B22" s="15">
+        <v>58</v>
+      </c>
+      <c r="C22" s="11">
+        <v>21</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
         <v>13</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15">
-        <v>77</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="B23" s="15">
+        <v>50</v>
+      </c>
+      <c r="C23" s="11">
+        <v>22</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>3</v>
-      </c>
-      <c r="B7" s="15">
-        <v>6</v>
-      </c>
-      <c r="C7" s="15" t="s">
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="15">
+        <v>54</v>
+      </c>
+      <c r="C24" s="11">
+        <v>23</v>
+      </c>
+      <c r="D24" s="11">
+        <v>58</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="15">
+        <v>56</v>
+      </c>
+      <c r="C25" s="11">
+        <v>24</v>
+      </c>
+      <c r="D25" s="11">
+        <v>81</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="15">
+        <v>53</v>
+      </c>
+      <c r="C26" s="11">
+        <v>25</v>
+      </c>
+      <c r="D26" s="11">
+        <v>82</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>14</v>
+      </c>
+      <c r="B27" s="15">
+        <v>18</v>
+      </c>
+      <c r="C27" s="11">
         <v>26</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>4</v>
-      </c>
-      <c r="B8" s="15">
-        <v>7</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="D27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="15">
+        <v>49</v>
+      </c>
+      <c r="C28" s="11">
+        <v>27</v>
+      </c>
+      <c r="D28" s="11">
+        <v>83</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
         <v>15</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15">
-        <v>18</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>5</v>
-      </c>
-      <c r="B10" s="15">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="15">
-        <v>10</v>
-      </c>
-      <c r="C11" s="15">
-        <v>27</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="B29" s="15">
+        <v>338</v>
+      </c>
+      <c r="C29" s="11">
+        <v>28</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>6</v>
-      </c>
-      <c r="B12" s="15">
-        <v>11</v>
-      </c>
-      <c r="C12" s="15" t="s">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="15">
+        <v>326</v>
+      </c>
+      <c r="C30" s="11">
+        <v>29</v>
+      </c>
+      <c r="D30" s="11">
+        <v>84</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
         <v>16</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15">
-        <v>12</v>
-      </c>
-      <c r="C13" s="15">
-        <v>78</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <v>7</v>
-      </c>
-      <c r="B14" s="15">
-        <v>13</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="B31" s="15">
+        <v>338</v>
+      </c>
+      <c r="C31" s="11">
+        <v>30</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="19">
         <v>17</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
-        <v>8</v>
-      </c>
-      <c r="B15" s="15">
-        <v>14</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15">
-        <v>15</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="B32" s="15">
+        <v>304</v>
+      </c>
+      <c r="C32" s="11">
+        <v>31</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="15">
+        <v>336</v>
+      </c>
+      <c r="C33" s="11">
+        <v>32</v>
+      </c>
+      <c r="D33" s="11">
+        <v>68</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>9</v>
-      </c>
-      <c r="B17" s="15">
-        <v>16</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <v>10</v>
-      </c>
-      <c r="B18" s="15">
-        <v>17</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15">
-        <v>18</v>
-      </c>
-      <c r="C19" s="15">
-        <v>79</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="15">
-        <v>19</v>
-      </c>
-      <c r="C20" s="15">
-        <v>80</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
-        <v>11</v>
-      </c>
-      <c r="B21" s="15">
-        <v>20</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <v>12</v>
-      </c>
-      <c r="B22" s="15">
-        <v>21</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>13</v>
-      </c>
-      <c r="B23" s="15">
-        <v>22</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15">
-        <v>23</v>
-      </c>
-      <c r="C24" s="15">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="15">
+        <v>308</v>
+      </c>
+      <c r="C34" s="11">
+        <v>33</v>
+      </c>
+      <c r="D34" s="11">
+        <v>85</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="15">
+        <v>312</v>
+      </c>
+      <c r="C35" s="11">
+        <v>34</v>
+      </c>
+      <c r="D35" s="11">
+        <v>86</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15">
-        <v>24</v>
-      </c>
-      <c r="C25" s="15">
-        <v>81</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15">
-        <v>25</v>
-      </c>
-      <c r="C26" s="15">
-        <v>82</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <v>14</v>
-      </c>
-      <c r="B27" s="15">
-        <v>26</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="15">
-        <v>27</v>
-      </c>
-      <c r="C28" s="15">
-        <v>83</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
-        <v>15</v>
-      </c>
-      <c r="B29" s="15">
-        <v>28</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="15">
-        <v>29</v>
-      </c>
-      <c r="C30" s="15">
-        <v>84</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
-        <v>16</v>
-      </c>
-      <c r="B31" s="15">
-        <v>30</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
-        <v>17</v>
-      </c>
-      <c r="B32" s="15">
-        <v>31</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="15">
-        <v>32</v>
-      </c>
-      <c r="C33" s="15">
-        <v>68</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="15">
-        <v>33</v>
-      </c>
-      <c r="C34" s="15">
-        <v>85</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="15">
-        <v>34</v>
-      </c>
-      <c r="C35" s="15">
-        <v>86</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
       <c r="B36" s="15">
+        <v>305</v>
+      </c>
+      <c r="C36" s="11">
         <v>35</v>
       </c>
-      <c r="C36" s="15">
+      <c r="D36" s="11">
         <v>87</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
+      <c r="E36" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:A6"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A32:A36"/>
@@ -2304,7 +2420,6 @@
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A4:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2315,8 +2430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,7 +2456,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2366,7 +2481,7 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2381,7 +2496,7 @@
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>81</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -2398,7 +2513,7 @@
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>79</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -2413,11 +2528,11 @@
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>76</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -2428,11 +2543,11 @@
       <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>75</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4"/>
     </row>
@@ -2443,11 +2558,11 @@
       <c r="B8" s="4">
         <v>6</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>72</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4">
         <v>72</v>
@@ -2460,11 +2575,11 @@
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -2475,154 +2590,154 @@
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>68</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>9</v>
+      </c>
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13">
+        <v>65</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>9</v>
-      </c>
-      <c r="B11" s="17">
-        <v>9</v>
-      </c>
-      <c r="C11" s="18">
-        <v>65</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13">
+        <v>63</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>10</v>
-      </c>
-      <c r="B12" s="17">
-        <v>10</v>
-      </c>
-      <c r="C12" s="18">
-        <v>63</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="13">
+        <v>59</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>11</v>
-      </c>
-      <c r="B13" s="17">
-        <v>11</v>
-      </c>
-      <c r="C13" s="18">
-        <v>59</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>12</v>
+      </c>
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="13">
+        <v>58</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>12</v>
-      </c>
-      <c r="B14" s="17">
-        <v>12</v>
-      </c>
-      <c r="C14" s="18">
-        <v>58</v>
-      </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>13</v>
+      </c>
+      <c r="B15" s="12">
+        <v>13</v>
+      </c>
+      <c r="C15" s="13">
+        <v>57</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>13</v>
-      </c>
-      <c r="B15" s="17">
-        <v>13</v>
-      </c>
-      <c r="C15" s="18">
+      <c r="E15" s="12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12">
+        <v>14</v>
+      </c>
+      <c r="C16" s="13">
+        <v>50</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>15</v>
+      </c>
+      <c r="B17" s="12">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13">
+        <v>17</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>16</v>
+      </c>
+      <c r="B18" s="12">
+        <v>16</v>
+      </c>
+      <c r="C18" s="13">
+        <v>338</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="17">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>14</v>
-      </c>
-      <c r="B16" s="17">
-        <v>14</v>
-      </c>
-      <c r="C16" s="18">
-        <v>50</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="17">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="17">
-        <v>15</v>
-      </c>
-      <c r="C17" s="18">
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
         <v>17</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="B19" s="12">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13">
+        <v>310</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>16</v>
-      </c>
-      <c r="B18" s="17">
-        <v>16</v>
-      </c>
-      <c r="C18" s="18">
-        <v>338</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <v>17</v>
-      </c>
-      <c r="B19" s="17">
-        <v>17</v>
-      </c>
-      <c r="C19" s="18">
-        <v>310</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -2692,19 +2807,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,13 +2893,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2795,7 +2910,7 @@
         <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2806,7 +2921,7 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2817,7 +2932,7 @@
         <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2828,7 +2943,7 @@
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,7 +2954,7 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2850,7 +2965,7 @@
         <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2861,7 +2976,7 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2872,7 +2987,7 @@
         <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2883,7 +2998,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2894,7 +3009,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2905,7 +3020,7 @@
         <v>339</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2916,7 +3031,7 @@
         <v>337</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2927,7 +3042,7 @@
         <v>312</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2938,7 +3053,7 @@
         <v>307</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2963,19 +3078,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
@@ -2992,7 +3107,7 @@
         <v>2918.55</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4">
         <v>81</v>
@@ -3012,7 +3127,7 @@
         <v>525.96</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="4">
         <v>81</v>
@@ -3032,7 +3147,7 @@
         <v>1340.21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="4">
         <v>77</v>
@@ -3052,7 +3167,7 @@
         <v>401.03</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="4">
         <v>74</v>
@@ -3072,7 +3187,7 @@
         <v>1120.05</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="4">
         <v>70</v>
@@ -3092,7 +3207,7 @@
         <v>580.23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4">
         <v>66</v>
@@ -3112,7 +3227,7 @@
         <v>1988.84</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4">
         <v>63</v>
@@ -3132,7 +3247,7 @@
         <v>1844.36</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4">
         <v>60</v>
@@ -3152,7 +3267,7 @@
         <v>431.99</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="4">
         <v>57</v>
@@ -3172,7 +3287,7 @@
         <v>780</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="4">
         <v>51</v>
@@ -3192,7 +3307,7 @@
         <v>309.56</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="4">
         <v>51</v>
@@ -3212,7 +3327,7 @@
         <v>906.31</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="4">
         <v>19</v>
@@ -3232,7 +3347,7 @@
         <v>248.54499999999999</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="4">
         <v>339</v>
@@ -3242,38 +3357,38 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="20">
         <v>13</v>
       </c>
       <c r="B15" s="4">
         <v>332</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="20">
         <v>761.25</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>49</v>
+      <c r="D15" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4">
         <v>335</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>336</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="4">
         <v>337</v>
       </c>
@@ -3292,7 +3407,7 @@
         <v>671.36</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="4">
         <v>311</v>
@@ -3312,7 +3427,7 @@
         <v>461.39299999999997</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="4">
         <v>307</v>
@@ -3332,7 +3447,7 @@
         <v>759.2</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="4">
         <v>307</v>
@@ -3357,256 +3472,257 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>82</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>78</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>71</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="F1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>82</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="B5" s="4">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>78</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="4">
+        <v>61</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>71</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6">
-        <v>61</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>54</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>49</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>7</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>600</v>
-      </c>
-    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="14">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>336</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <v>8</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
         <v>400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>